<commit_message>
Updated stories and story points
</commit_message>
<xml_diff>
--- a/Project3Requirements/User Stories and Future Stories.xlsx
+++ b/Project3Requirements/User Stories and Future Stories.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11018"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="174" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34839C68-27AE-4B11-BCAD-64AD1A20D4CC}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brettbalquist/KU-2025-2026/2025/EECS-581/Project-3-EECS581/Project3Requirements/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FB1CCB-B78E-AD46-8600-804ABFEFC456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Story References" sheetId="1" r:id="rId1"/>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
   <si>
     <t>Pool Story Points</t>
   </si>
@@ -163,77 +168,122 @@
     <t>Sprint No.</t>
   </si>
   <si>
-    <t>Set up the MERN project skeleton, including Node.js backend, Express routing, React frontend, and MongoDB connection. Establish the folder structure for scalability.</t>
-  </si>
-  <si>
-    <t>Initialize GitHub repository, implement branch protection rules, and configure automated builds with GitHub Actions for CI/CD testing.</t>
-  </si>
-  <si>
-    <t>Create .env configuration for sensitive keys, connect backend to MongoDB Atlas, and ensure secure environment setup.</t>
-  </si>
-  <si>
-    <t>Develop the initial React frontend with Tailwind CSS, reusable components, and responsive navigation layout.</t>
-  </si>
-  <si>
-    <t>Implement API base routes for testing connectivity (health check, status route) and confirm data flow between client and server.</t>
-  </si>
-  <si>
-    <t>Implement JWT-based authentication system for user signup, login, and token verification using bcrypt for password hashing.</t>
-  </si>
-  <si>
-    <t>Build user profile dashboard displaying streaks, completed challenges, and basic stats fetched from MongoDB.</t>
-  </si>
-  <si>
-    <t>Develop backend logic to release one new coding problem daily and lock it after 24 hours to simulate Wordle-style gameplay.</t>
-  </si>
-  <si>
-    <t>Create frontend interface for daily challenge with a timer, submit button, and progress tracker.</t>
-  </si>
-  <si>
-    <t>Implement backend endpoints for evaluating code submissions with pre-stored test cases and providing real-time feedback.</t>
-  </si>
-  <si>
-    <t>Integrate Monaco Editor for in-browser coding, including syntax highlighting and language support.</t>
-  </si>
-  <si>
-    <t>Add leaderboard with dynamic ranking based on user streaks, accuracy, and challenge completion time.</t>
-  </si>
-  <si>
-    <t>Implement difficulty tagging (Easy, Medium, Hard) and allow the admin to assign tags to each problem.</t>
-  </si>
-  <si>
-    <t>Build an admin dashboard to manage questions (CRUD operations), view user progress, and push new challenges.</t>
-  </si>
-  <si>
-    <t>Add streak tracker logic on backend and frontend with persistent daily login detection.</t>
-  </si>
-  <si>
-    <t>Implement reward badges and achievements (e.g., “7-day streak”, “10 correct in a row”) for user engagement.</t>
-  </si>
-  <si>
-    <t>Add hint system allowing users to reveal partial hints or full solutions after submission.</t>
-  </si>
-  <si>
-    <t>Integrate social sharing features for users to share daily results on Twitter/X and LinkedIn.</t>
-  </si>
-  <si>
-    <t>Conduct performance optimizations (lazy loading, caching, compression) to improve app speed and mobile experience.</t>
-  </si>
-  <si>
-    <t>Deploy full app using Render/Vercel for frontend and MongoDB Atlas for database. Ensure HTTPS and DNS setup.</t>
-  </si>
-  <si>
-    <t>Gather beta user feedback, document issues, and iterate improvements before presentation.</t>
-  </si>
-  <si>
-    <t>Finalize UI, fix bugs, conduct regression testing, and prepare demo presentation deck and walkthrough video.</t>
+    <t>Set up Node.js backend with Express routing</t>
+  </si>
+  <si>
+    <t>Set up React frontend with Tailwind CSS and responsive navigation</t>
+  </si>
+  <si>
+    <t>Connect backend to MongoDB and verify local connection</t>
+  </si>
+  <si>
+    <t>Establish folder structure for scalability and modularity</t>
+  </si>
+  <si>
+    <t>Initialize GitHub repository and add branch protection rules</t>
+  </si>
+  <si>
+    <t>Configure GitHub Actions for CI/CD builds</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>.env</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> configuration for sensitive keys</t>
+    </r>
+  </si>
+  <si>
+    <t>Implement API base routes for health check and status</t>
+  </si>
+  <si>
+    <t>Develop initial reusable React components</t>
+  </si>
+  <si>
+    <t>Ensure secure environment setup for backend</t>
+  </si>
+  <si>
+    <t>Implement JWT-based authentication system for signup/login</t>
+  </si>
+  <si>
+    <t>Add bcrypt password hashing for user security</t>
+  </si>
+  <si>
+    <t>Build user profile dashboard with streaks and basic stats</t>
+  </si>
+  <si>
+    <t>Develop backend logic for daily coding problem release and lock</t>
+  </si>
+  <si>
+    <t>Create frontend interface for daily challenge with timer</t>
+  </si>
+  <si>
+    <t>Implement backend endpoints to evaluate code submissions</t>
+  </si>
+  <si>
+    <t>Integrate Monaco Editor for in-browser coding with syntax highlighting</t>
+  </si>
+  <si>
+    <t>Add leaderboard with dynamic ranking based on streaks and accuracy</t>
+  </si>
+  <si>
+    <t>Implement difficulty tagging (Easy, Medium, Hard) for challenges</t>
+  </si>
+  <si>
+    <t>Build admin dashboard for CRUD on questions and user progress</t>
+  </si>
+  <si>
+    <t>Add streak tracker logic on backend and frontend</t>
+  </si>
+  <si>
+    <t>Conduct testing of Monaco Editor integration and debugging</t>
+  </si>
+  <si>
+    <t>Implement reward badges and achievements (e.g., 7-day streak)</t>
+  </si>
+  <si>
+    <t>Add hint system to reveal partial hints or full solutions</t>
+  </si>
+  <si>
+    <t>Integrate social sharing for daily results on Twitter/X and LinkedIn</t>
+  </si>
+  <si>
+    <t>Conduct performance optimizations (lazy loading, caching, compression)</t>
+  </si>
+  <si>
+    <t>Deploy full app using Render/Vercel with HTTPS and DNS setup</t>
+  </si>
+  <si>
+    <t>Gather beta user feedback, document issues, iterate improvements</t>
+  </si>
+  <si>
+    <t>Finalize UI, fix bugs, regression testing, prepare demo presentation</t>
+  </si>
+  <si>
+    <t>Write documentation for features, architecture, and deployment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,7 +304,20 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -277,10 +340,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,20 +681,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="87.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="87.5" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -644,7 +708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -658,7 +722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -672,9 +736,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -686,9 +750,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -700,7 +764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -714,9 +778,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -728,7 +792,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -742,9 +806,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -756,9 +820,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -770,7 +834,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>5</v>
       </c>
@@ -784,9 +848,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -798,9 +862,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -812,7 +876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>8</v>
       </c>
@@ -826,9 +890,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -840,9 +904,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -854,9 +918,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -868,9 +932,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
@@ -882,9 +946,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -896,7 +960,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>13</v>
       </c>
@@ -910,7 +974,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>5</v>
       </c>
@@ -924,7 +988,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>5</v>
       </c>
@@ -938,9 +1002,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -952,9 +1016,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -966,7 +1030,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>5</v>
       </c>
@@ -987,39 +1051,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C05C448-34C9-4BDB-9520-B326A466A8B6}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="152.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="152.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1036,7 +1100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -1044,7 +1108,7 @@
         <v>44</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1053,7 +1117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1.2</v>
       </c>
@@ -1070,7 +1134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1.3</v>
       </c>
@@ -1078,7 +1142,7 @@
         <v>46</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -1087,7 +1151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1.4</v>
       </c>
@@ -1095,7 +1159,7 @@
         <v>47</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1104,60 +1168,60 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2.1</v>
+        <v>1.6</v>
       </c>
       <c r="B8" t="s">
         <v>49</v>
       </c>
       <c r="C8">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
       <c r="B9" t="s">
         <v>50</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2.2999999999999998</v>
+        <v>1.8</v>
       </c>
       <c r="B10" t="s">
         <v>51</v>
@@ -1169,97 +1233,97 @@
         <v>9</v>
       </c>
       <c r="E10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2.4</v>
+        <v>1.9</v>
       </c>
       <c r="B11" t="s">
         <v>52</v>
       </c>
       <c r="C11">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>53</v>
       </c>
       <c r="C12">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <v>11</v>
       </c>
       <c r="E12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="B13" t="s">
         <v>54</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>12</v>
       </c>
       <c r="E13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>3.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B14" t="s">
         <v>55</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>13</v>
       </c>
       <c r="E14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>3.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B15" t="s">
         <v>56</v>
       </c>
       <c r="C15">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D15">
         <v>14</v>
       </c>
       <c r="E15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>3.4</v>
+        <v>2.4</v>
       </c>
       <c r="B16" t="s">
         <v>57</v>
@@ -1271,63 +1335,63 @@
         <v>15</v>
       </c>
       <c r="E16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="B17" t="s">
         <v>58</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D17">
         <v>16</v>
       </c>
       <c r="E17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>4.0999999999999996</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
         <v>59</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D18">
         <v>17</v>
       </c>
       <c r="E18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>4.2</v>
+        <v>3.1</v>
       </c>
       <c r="B19" t="s">
         <v>60</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>18</v>
       </c>
       <c r="E19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>4.3</v>
+        <v>3.2</v>
       </c>
       <c r="B20" t="s">
         <v>61</v>
@@ -1339,57 +1403,193 @@
         <v>19</v>
       </c>
       <c r="E20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>4.4000000000000004</v>
+        <v>3.3</v>
       </c>
       <c r="B21" t="s">
         <v>62</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D21">
         <v>20</v>
       </c>
       <c r="E21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>4.5</v>
+        <v>3.4</v>
       </c>
       <c r="B22" t="s">
         <v>63</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D22">
         <v>21</v>
       </c>
       <c r="E22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>4.5999999999999996</v>
+        <v>3.5</v>
       </c>
       <c r="B23" t="s">
         <v>64</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D23">
         <v>22</v>
       </c>
       <c r="E23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>23</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>24</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>4.2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>4.3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>26</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>27</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>4.5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>28</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>29</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>4.7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+      <c r="E31">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated for flask instead of MERN
</commit_message>
<xml_diff>
--- a/Project3Requirements/User Stories and Future Stories.xlsx
+++ b/Project3Requirements/User Stories and Future Stories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brettbalquist/KU-2025-2026/2025/EECS-581/Project-3-EECS581/Project3Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FB1CCB-B78E-AD46-8600-804ABFEFC456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5FBEA5-4FDF-AF47-815E-62F7F4FC654F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Story References" sheetId="1" r:id="rId1"/>
@@ -1054,7 +1054,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated All sprint Artifacts and Excel Document based on changes
</commit_message>
<xml_diff>
--- a/Project3Requirements/User Stories and Future Stories.xlsx
+++ b/Project3Requirements/User Stories and Future Stories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brettbalquist/KU-2025-2026/2025/EECS-581/Project-3-EECS581/Project3Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5FBEA5-4FDF-AF47-815E-62F7F4FC654F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB19931-C2DD-6E47-B129-8511CD1A86E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="760" windowWidth="29040" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Story References" sheetId="1" r:id="rId1"/>
@@ -168,15 +168,6 @@
     <t>Sprint No.</t>
   </si>
   <si>
-    <t>Set up Node.js backend with Express routing</t>
-  </si>
-  <si>
-    <t>Set up React frontend with Tailwind CSS and responsive navigation</t>
-  </si>
-  <si>
-    <t>Connect backend to MongoDB and verify local connection</t>
-  </si>
-  <si>
     <t>Establish folder structure for scalability and modularity</t>
   </si>
   <si>
@@ -186,30 +177,6 @@
     <t>Configure GitHub Actions for CI/CD builds</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Create </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>.env</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> configuration for sensitive keys</t>
-    </r>
-  </si>
-  <si>
     <t>Implement API base routes for health check and status</t>
   </si>
   <si>
@@ -277,13 +244,25 @@
   </si>
   <si>
     <t>Write documentation for features, architecture, and deployment</t>
+  </si>
+  <si>
+    <t>Set up Python backend with Flask</t>
+  </si>
+  <si>
+    <t>Set up React frontend with Vite, Tailwind CSS, and responsive navigation</t>
+  </si>
+  <si>
+    <t>Connect backend to SQLite and verify local connection</t>
+  </si>
+  <si>
+    <t>Create .env configuration for sensitive keys</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,12 +291,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1054,7 +1027,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1088,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -1105,7 +1078,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -1122,7 +1095,7 @@
         <v>1.2</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1139,7 +1112,7 @@
         <v>1.3</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -1156,7 +1129,7 @@
         <v>1.4</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1173,7 +1146,7 @@
         <v>1.5</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1185,12 +1158,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1.6</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1207,7 +1180,7 @@
         <v>1.7</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1224,7 +1197,7 @@
         <v>1.8</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -1241,7 +1214,7 @@
         <v>1.9</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -1258,7 +1231,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C12">
         <v>8</v>
@@ -1275,7 +1248,7 @@
         <v>2.1</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -1292,7 +1265,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C14">
         <v>8</v>
@@ -1309,7 +1282,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -1326,7 +1299,7 @@
         <v>2.4</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -1343,7 +1316,7 @@
         <v>2.5</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C17">
         <v>13</v>
@@ -1360,7 +1333,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C18">
         <v>13</v>
@@ -1377,7 +1350,7 @@
         <v>3.1</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -1394,7 +1367,7 @@
         <v>3.2</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -1411,7 +1384,7 @@
         <v>3.3</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C21">
         <v>8</v>
@@ -1428,7 +1401,7 @@
         <v>3.4</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -1445,7 +1418,7 @@
         <v>3.5</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -1462,7 +1435,7 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -1479,7 +1452,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -1496,7 +1469,7 @@
         <v>4.2</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -1513,7 +1486,7 @@
         <v>4.3</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -1530,7 +1503,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -1547,7 +1520,7 @@
         <v>4.5</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C29">
         <v>5</v>
@@ -1564,7 +1537,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C30">
         <v>5</v>
@@ -1581,7 +1554,7 @@
         <v>4.7</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C31">
         <v>3</v>

</xml_diff>